<commit_message>
Fix failing tests + add more test for referral network graph output + add format settings for replay mode : e.g. gpgk, tif, instead of shapefile and HFa img
</commit_message>
<xml_diff>
--- a/tests/referral/data/result_conf_init.xlsx
+++ b/tests/referral/data/result_conf_init.xlsx
@@ -1,52 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t xml:space="preserve">from__cat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from__name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to__cat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to__name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">distance_km</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time_m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chabvala Health Centre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chipini Rural Hospital</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -72,13 +52,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -128,6 +112,10 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -153,12 +141,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -184,7 +175,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -360,75 +350,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>from__cat</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>from__name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>to__cat</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>to__name</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>distance_km</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>time_m</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Chabvala Health Centre</t>
+        </is>
+      </c>
+      <c r="C2">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Chipini Rural Hospital</t>
+        </is>
+      </c>
+      <c r="E2">
         <v>73</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>704</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="n">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Chipini Rural Hospital</t>
+        </is>
+      </c>
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Chabvala Health Centre</t>
+        </is>
+      </c>
+      <c r="E3">
         <v>73</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>650</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>